<commit_message>
upload to create an event works, uploading to update an event makes new event so hidden for now
</commit_message>
<xml_diff>
--- a/public/Seat Data Report.xlsx
+++ b/public/Seat Data Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qiyinyao/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joseph\EventNXT-606\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E3A5C5-7C2F-F046-ACFD-2D04CC71EF63}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{592308F7-33E4-4E06-AE71-B189D49A4702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9900" yWindow="1200" windowWidth="25600" windowHeight="19020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5336" uniqueCount="988">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5336" uniqueCount="987">
   <si>
     <t>Purchased</t>
   </si>
@@ -2981,10 +2981,6 @@
   </si>
   <si>
     <t>sec: A row: 4 seat: 44</t>
-  </si>
-  <si>
-    <t>2019 FashioNXT Week Runway Shows - October 2nd</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2992,7 +2988,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="[$$-45C]\ #,##0.00_-"/>
+    <numFmt numFmtId="164" formatCode="[$$-45C]\ #,##0.00_-"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -3037,18 +3033,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -3064,7 +3057,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3362,42 +3355,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y432"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" customWidth="1"/>
     <col min="3" max="3" width="54" customWidth="1"/>
-    <col min="4" max="4" width="39.1640625" customWidth="1"/>
-    <col min="5" max="5" width="16.1640625" customWidth="1"/>
+    <col min="4" max="4" width="39.109375" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" customWidth="1"/>
     <col min="6" max="6" width="29.6640625" customWidth="1"/>
-    <col min="7" max="7" width="13.5" customWidth="1"/>
-    <col min="8" max="8" width="9.5" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" customWidth="1"/>
+    <col min="8" max="8" width="9.44140625" customWidth="1"/>
     <col min="9" max="9" width="23" customWidth="1"/>
-    <col min="10" max="10" width="20.1640625" customWidth="1"/>
+    <col min="10" max="10" width="20.109375" customWidth="1"/>
     <col min="11" max="11" width="24.33203125" customWidth="1"/>
-    <col min="12" max="12" width="16.1640625" customWidth="1"/>
-    <col min="13" max="13" width="10.83203125" customWidth="1"/>
-    <col min="14" max="14" width="16.1640625" customWidth="1"/>
+    <col min="12" max="12" width="16.109375" customWidth="1"/>
+    <col min="13" max="13" width="10.77734375" customWidth="1"/>
+    <col min="14" max="14" width="16.109375" customWidth="1"/>
     <col min="15" max="15" width="54" customWidth="1"/>
-    <col min="16" max="16" width="16.1640625" customWidth="1"/>
+    <col min="16" max="16" width="16.109375" customWidth="1"/>
     <col min="17" max="17" width="24.33203125" customWidth="1"/>
     <col min="18" max="18" width="29.6640625" customWidth="1"/>
-    <col min="19" max="19" width="44.5" customWidth="1"/>
-    <col min="20" max="20" width="16.1640625" customWidth="1"/>
+    <col min="19" max="19" width="44.44140625" customWidth="1"/>
+    <col min="20" max="20" width="16.109375" customWidth="1"/>
     <col min="21" max="21" width="6.6640625" customWidth="1"/>
-    <col min="22" max="22" width="13.5" customWidth="1"/>
-    <col min="23" max="23" width="18.83203125" customWidth="1"/>
-    <col min="24" max="24" width="37.83203125" customWidth="1"/>
-    <col min="25" max="25" width="12.1640625" customWidth="1"/>
+    <col min="22" max="22" width="13.44140625" customWidth="1"/>
+    <col min="23" max="23" width="18.77734375" customWidth="1"/>
+    <col min="24" max="24" width="37.77734375" customWidth="1"/>
+    <col min="25" max="25" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="15">
-      <c r="A1" s="5" t="s">
-        <v>987</v>
+    <row r="1" spans="1:25">
+      <c r="A1" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -3424,7 +3415,7 @@
       <c r="X1" s="4"/>
       <c r="Y1" s="4"/>
     </row>
-    <row r="2" spans="1:25" ht="15">
+    <row r="2" spans="1:25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3501,7 +3492,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="15">
+    <row r="3" spans="1:25">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -3548,7 +3539,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="15">
+    <row r="4" spans="1:25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -3595,7 +3586,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="15">
+    <row r="5" spans="1:25">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -3642,7 +3633,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="15">
+    <row r="6" spans="1:25">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -3689,7 +3680,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="15">
+    <row r="7" spans="1:25">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -3736,7 +3727,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="15">
+    <row r="8" spans="1:25">
       <c r="A8" t="s">
         <v>49</v>
       </c>
@@ -3792,7 +3783,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="15">
+    <row r="9" spans="1:25">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -3848,7 +3839,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="15">
+    <row r="10" spans="1:25">
       <c r="A10" t="s">
         <v>60</v>
       </c>
@@ -3907,7 +3898,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="15">
+    <row r="11" spans="1:25">
       <c r="A11" t="s">
         <v>71</v>
       </c>
@@ -3951,7 +3942,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="15">
+    <row r="12" spans="1:25">
       <c r="A12" t="s">
         <v>75</v>
       </c>
@@ -3998,7 +3989,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="15">
+    <row r="13" spans="1:25">
       <c r="A13" t="s">
         <v>75</v>
       </c>
@@ -4045,7 +4036,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="15">
+    <row r="14" spans="1:25">
       <c r="A14" t="s">
         <v>80</v>
       </c>
@@ -4092,7 +4083,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="15">
+    <row r="15" spans="1:25">
       <c r="A15" t="s">
         <v>80</v>
       </c>
@@ -4139,7 +4130,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="15">
+    <row r="16" spans="1:25">
       <c r="A16" t="s">
         <v>87</v>
       </c>
@@ -4183,7 +4174,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="15">
+    <row r="17" spans="1:25">
       <c r="A17" t="s">
         <v>90</v>
       </c>
@@ -4230,7 +4221,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="15">
+    <row r="18" spans="1:25">
       <c r="A18" t="s">
         <v>94</v>
       </c>
@@ -4277,7 +4268,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="15">
+    <row r="19" spans="1:25">
       <c r="A19" t="s">
         <v>97</v>
       </c>
@@ -4324,7 +4315,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="15">
+    <row r="20" spans="1:25">
       <c r="A20" t="s">
         <v>97</v>
       </c>
@@ -4371,7 +4362,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="15">
+    <row r="21" spans="1:25">
       <c r="A21" t="s">
         <v>102</v>
       </c>
@@ -4430,7 +4421,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="15">
+    <row r="22" spans="1:25">
       <c r="A22" t="s">
         <v>111</v>
       </c>
@@ -4477,7 +4468,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="15">
+    <row r="23" spans="1:25">
       <c r="A23" t="s">
         <v>111</v>
       </c>
@@ -4524,7 +4515,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="24" spans="1:25" ht="15">
+    <row r="24" spans="1:25">
       <c r="A24" t="s">
         <v>117</v>
       </c>
@@ -4571,7 +4562,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="25" spans="1:25" ht="15">
+    <row r="25" spans="1:25">
       <c r="A25" t="s">
         <v>117</v>
       </c>
@@ -4618,7 +4609,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="26" spans="1:25" ht="15">
+    <row r="26" spans="1:25">
       <c r="A26" t="s">
         <v>117</v>
       </c>
@@ -4665,7 +4656,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="27" spans="1:25" ht="15">
+    <row r="27" spans="1:25">
       <c r="A27" t="s">
         <v>117</v>
       </c>
@@ -4712,7 +4703,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="28" spans="1:25" ht="15">
+    <row r="28" spans="1:25">
       <c r="A28" t="s">
         <v>117</v>
       </c>
@@ -4759,7 +4750,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="29" spans="1:25" ht="15">
+    <row r="29" spans="1:25">
       <c r="A29" t="s">
         <v>117</v>
       </c>
@@ -4806,7 +4797,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="30" spans="1:25" ht="15">
+    <row r="30" spans="1:25">
       <c r="A30" t="s">
         <v>117</v>
       </c>
@@ -4853,7 +4844,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="31" spans="1:25" ht="15">
+    <row r="31" spans="1:25">
       <c r="A31" t="s">
         <v>127</v>
       </c>
@@ -4900,7 +4891,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="32" spans="1:25" ht="15">
+    <row r="32" spans="1:25">
       <c r="A32" t="s">
         <v>127</v>
       </c>
@@ -4947,7 +4938,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="33" spans="1:25" ht="15">
+    <row r="33" spans="1:25">
       <c r="A33" t="s">
         <v>132</v>
       </c>
@@ -5006,7 +4997,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="1:25" ht="15">
+    <row r="34" spans="1:25">
       <c r="A34" t="s">
         <v>140</v>
       </c>
@@ -5056,7 +5047,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="1:25" ht="15">
+    <row r="35" spans="1:25">
       <c r="A35" t="s">
         <v>147</v>
       </c>
@@ -5103,7 +5094,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="36" spans="1:25" ht="15">
+    <row r="36" spans="1:25">
       <c r="A36" t="s">
         <v>147</v>
       </c>
@@ -5150,7 +5141,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="37" spans="1:25" ht="15">
+    <row r="37" spans="1:25">
       <c r="A37" t="s">
         <v>152</v>
       </c>
@@ -5209,7 +5200,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="38" spans="1:25" ht="15">
+    <row r="38" spans="1:25">
       <c r="A38" t="s">
         <v>160</v>
       </c>
@@ -5268,7 +5259,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="39" spans="1:25" ht="15">
+    <row r="39" spans="1:25">
       <c r="A39" t="s">
         <v>169</v>
       </c>
@@ -5327,7 +5318,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="1:25" ht="15">
+    <row r="40" spans="1:25">
       <c r="A40" t="s">
         <v>176</v>
       </c>
@@ -5371,7 +5362,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="41" spans="1:25" ht="15">
+    <row r="41" spans="1:25">
       <c r="A41" t="s">
         <v>176</v>
       </c>
@@ -5415,7 +5406,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="42" spans="1:25" ht="15">
+    <row r="42" spans="1:25">
       <c r="A42" t="s">
         <v>176</v>
       </c>
@@ -5459,7 +5450,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="43" spans="1:25" ht="15">
+    <row r="43" spans="1:25">
       <c r="A43" t="s">
         <v>181</v>
       </c>
@@ -5506,7 +5497,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="44" spans="1:25" ht="15">
+    <row r="44" spans="1:25">
       <c r="A44" t="s">
         <v>185</v>
       </c>
@@ -5553,7 +5544,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="45" spans="1:25" ht="15">
+    <row r="45" spans="1:25">
       <c r="A45" t="s">
         <v>185</v>
       </c>
@@ -5600,7 +5591,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="46" spans="1:25" ht="15">
+    <row r="46" spans="1:25">
       <c r="A46" t="s">
         <v>185</v>
       </c>
@@ -5647,7 +5638,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="47" spans="1:25" ht="15">
+    <row r="47" spans="1:25">
       <c r="A47" t="s">
         <v>193</v>
       </c>
@@ -5694,7 +5685,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="48" spans="1:25" ht="15">
+    <row r="48" spans="1:25">
       <c r="A48" t="s">
         <v>193</v>
       </c>
@@ -5741,7 +5732,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="49" spans="1:25" ht="15">
+    <row r="49" spans="1:25">
       <c r="A49" t="s">
         <v>193</v>
       </c>
@@ -5788,7 +5779,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="50" spans="1:25" ht="15">
+    <row r="50" spans="1:25">
       <c r="A50" t="s">
         <v>193</v>
       </c>
@@ -5835,7 +5826,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="51" spans="1:25" ht="15">
+    <row r="51" spans="1:25">
       <c r="A51" t="s">
         <v>201</v>
       </c>
@@ -5888,7 +5879,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="52" spans="1:25" ht="15">
+    <row r="52" spans="1:25">
       <c r="A52" t="s">
         <v>209</v>
       </c>
@@ -5935,7 +5926,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="53" spans="1:25" ht="15">
+    <row r="53" spans="1:25">
       <c r="A53" t="s">
         <v>209</v>
       </c>
@@ -5982,7 +5973,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="54" spans="1:25" ht="15">
+    <row r="54" spans="1:25">
       <c r="A54" t="s">
         <v>214</v>
       </c>
@@ -6029,7 +6020,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="55" spans="1:25" ht="15">
+    <row r="55" spans="1:25">
       <c r="A55" t="s">
         <v>214</v>
       </c>
@@ -6076,7 +6067,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="56" spans="1:25" ht="15">
+    <row r="56" spans="1:25">
       <c r="A56" t="s">
         <v>214</v>
       </c>
@@ -6123,7 +6114,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="57" spans="1:25" ht="15">
+    <row r="57" spans="1:25">
       <c r="A57" t="s">
         <v>214</v>
       </c>
@@ -6170,7 +6161,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="58" spans="1:25" ht="15">
+    <row r="58" spans="1:25">
       <c r="A58" t="s">
         <v>214</v>
       </c>
@@ -6217,7 +6208,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="59" spans="1:25" ht="15">
+    <row r="59" spans="1:25">
       <c r="A59" t="s">
         <v>214</v>
       </c>
@@ -6264,7 +6255,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="60" spans="1:25" ht="15">
+    <row r="60" spans="1:25">
       <c r="A60" t="s">
         <v>214</v>
       </c>
@@ -6311,7 +6302,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="61" spans="1:25" ht="15">
+    <row r="61" spans="1:25">
       <c r="A61" t="s">
         <v>214</v>
       </c>
@@ -6358,7 +6349,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="62" spans="1:25" ht="15">
+    <row r="62" spans="1:25">
       <c r="A62" t="s">
         <v>214</v>
       </c>
@@ -6405,7 +6396,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="63" spans="1:25" ht="15">
+    <row r="63" spans="1:25">
       <c r="A63" t="s">
         <v>214</v>
       </c>
@@ -6452,7 +6443,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="64" spans="1:25" ht="15">
+    <row r="64" spans="1:25">
       <c r="A64" t="s">
         <v>214</v>
       </c>
@@ -6499,7 +6490,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="65" spans="1:22" ht="15">
+    <row r="65" spans="1:22">
       <c r="A65" t="s">
         <v>214</v>
       </c>
@@ -6546,7 +6537,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="66" spans="1:22" ht="15">
+    <row r="66" spans="1:22">
       <c r="A66" t="s">
         <v>214</v>
       </c>
@@ -6593,7 +6584,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="67" spans="1:22" ht="15">
+    <row r="67" spans="1:22">
       <c r="A67" t="s">
         <v>214</v>
       </c>
@@ -6640,7 +6631,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="68" spans="1:22" ht="15">
+    <row r="68" spans="1:22">
       <c r="A68" t="s">
         <v>214</v>
       </c>
@@ -6687,7 +6678,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="69" spans="1:22" ht="15">
+    <row r="69" spans="1:22">
       <c r="A69" t="s">
         <v>214</v>
       </c>
@@ -6734,7 +6725,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="70" spans="1:22" ht="15">
+    <row r="70" spans="1:22">
       <c r="A70" t="s">
         <v>214</v>
       </c>
@@ -6781,7 +6772,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="71" spans="1:22" ht="15">
+    <row r="71" spans="1:22">
       <c r="A71" t="s">
         <v>214</v>
       </c>
@@ -6828,7 +6819,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="72" spans="1:22" ht="15">
+    <row r="72" spans="1:22">
       <c r="A72" t="s">
         <v>214</v>
       </c>
@@ -6875,7 +6866,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="73" spans="1:22" ht="15">
+    <row r="73" spans="1:22">
       <c r="A73" t="s">
         <v>214</v>
       </c>
@@ -6922,7 +6913,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="74" spans="1:22" ht="15">
+    <row r="74" spans="1:22">
       <c r="A74" t="s">
         <v>214</v>
       </c>
@@ -6969,7 +6960,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="75" spans="1:22" ht="15">
+    <row r="75" spans="1:22">
       <c r="A75" t="s">
         <v>214</v>
       </c>
@@ -7016,7 +7007,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="76" spans="1:22" ht="15">
+    <row r="76" spans="1:22">
       <c r="A76" t="s">
         <v>214</v>
       </c>
@@ -7063,7 +7054,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="77" spans="1:22" ht="15">
+    <row r="77" spans="1:22">
       <c r="A77" t="s">
         <v>214</v>
       </c>
@@ -7110,7 +7101,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="78" spans="1:22" ht="15">
+    <row r="78" spans="1:22">
       <c r="A78" t="s">
         <v>214</v>
       </c>
@@ -7157,7 +7148,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="79" spans="1:22" ht="15">
+    <row r="79" spans="1:22">
       <c r="A79" t="s">
         <v>214</v>
       </c>
@@ -7204,7 +7195,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="80" spans="1:22" ht="15">
+    <row r="80" spans="1:22">
       <c r="A80" t="s">
         <v>214</v>
       </c>
@@ -7251,7 +7242,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="81" spans="1:22" ht="15">
+    <row r="81" spans="1:22">
       <c r="A81" t="s">
         <v>214</v>
       </c>
@@ -7298,7 +7289,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="82" spans="1:22" ht="15">
+    <row r="82" spans="1:22">
       <c r="A82" t="s">
         <v>214</v>
       </c>
@@ -7345,7 +7336,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="83" spans="1:22" ht="15">
+    <row r="83" spans="1:22">
       <c r="A83" t="s">
         <v>214</v>
       </c>
@@ -7392,7 +7383,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="84" spans="1:22" ht="15">
+    <row r="84" spans="1:22">
       <c r="A84" t="s">
         <v>214</v>
       </c>
@@ -7439,7 +7430,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="85" spans="1:22" ht="15">
+    <row r="85" spans="1:22">
       <c r="A85" t="s">
         <v>214</v>
       </c>
@@ -7486,7 +7477,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="86" spans="1:22" ht="15">
+    <row r="86" spans="1:22">
       <c r="A86" t="s">
         <v>214</v>
       </c>
@@ -7533,7 +7524,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="87" spans="1:22" ht="15">
+    <row r="87" spans="1:22">
       <c r="A87" t="s">
         <v>214</v>
       </c>
@@ -7580,7 +7571,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="88" spans="1:22" ht="15">
+    <row r="88" spans="1:22">
       <c r="A88" t="s">
         <v>214</v>
       </c>
@@ -7627,7 +7618,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="89" spans="1:22" ht="15">
+    <row r="89" spans="1:22">
       <c r="A89" t="s">
         <v>214</v>
       </c>
@@ -7674,7 +7665,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="90" spans="1:22" ht="15">
+    <row r="90" spans="1:22">
       <c r="A90" t="s">
         <v>214</v>
       </c>
@@ -7721,7 +7712,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="91" spans="1:22" ht="15">
+    <row r="91" spans="1:22">
       <c r="A91" t="s">
         <v>214</v>
       </c>
@@ -7768,7 +7759,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="92" spans="1:22" ht="15">
+    <row r="92" spans="1:22">
       <c r="A92" t="s">
         <v>214</v>
       </c>
@@ -7815,7 +7806,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="93" spans="1:22" ht="15">
+    <row r="93" spans="1:22">
       <c r="A93" t="s">
         <v>214</v>
       </c>
@@ -7862,7 +7853,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="94" spans="1:22" ht="15">
+    <row r="94" spans="1:22">
       <c r="A94" t="s">
         <v>214</v>
       </c>
@@ -7909,7 +7900,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="95" spans="1:22" ht="15">
+    <row r="95" spans="1:22">
       <c r="A95" t="s">
         <v>214</v>
       </c>
@@ -7956,7 +7947,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="96" spans="1:22" ht="15">
+    <row r="96" spans="1:22">
       <c r="A96" t="s">
         <v>214</v>
       </c>
@@ -8003,7 +7994,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="97" spans="1:22" ht="15">
+    <row r="97" spans="1:22">
       <c r="A97" t="s">
         <v>214</v>
       </c>
@@ -8050,7 +8041,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="98" spans="1:22" ht="15">
+    <row r="98" spans="1:22">
       <c r="A98" t="s">
         <v>260</v>
       </c>
@@ -8097,7 +8088,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="99" spans="1:22" ht="15">
+    <row r="99" spans="1:22">
       <c r="A99" t="s">
         <v>260</v>
       </c>
@@ -8144,7 +8135,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="100" spans="1:22" ht="15">
+    <row r="100" spans="1:22">
       <c r="A100" t="s">
         <v>260</v>
       </c>
@@ -8191,7 +8182,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="101" spans="1:22" ht="15">
+    <row r="101" spans="1:22">
       <c r="A101" t="s">
         <v>260</v>
       </c>
@@ -8238,7 +8229,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="102" spans="1:22" ht="15">
+    <row r="102" spans="1:22">
       <c r="A102" t="s">
         <v>260</v>
       </c>
@@ -8285,7 +8276,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="103" spans="1:22" ht="15">
+    <row r="103" spans="1:22">
       <c r="A103" t="s">
         <v>260</v>
       </c>
@@ -8332,7 +8323,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="104" spans="1:22" ht="15">
+    <row r="104" spans="1:22">
       <c r="A104" t="s">
         <v>260</v>
       </c>
@@ -8379,7 +8370,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="105" spans="1:22" ht="15">
+    <row r="105" spans="1:22">
       <c r="A105" t="s">
         <v>260</v>
       </c>
@@ -8426,7 +8417,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="106" spans="1:22" ht="15">
+    <row r="106" spans="1:22">
       <c r="A106" t="s">
         <v>260</v>
       </c>
@@ -8473,7 +8464,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="107" spans="1:22" ht="15">
+    <row r="107" spans="1:22">
       <c r="A107" t="s">
         <v>260</v>
       </c>
@@ -8520,7 +8511,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="108" spans="1:22" ht="15">
+    <row r="108" spans="1:22">
       <c r="A108" t="s">
         <v>260</v>
       </c>
@@ -8567,7 +8558,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="109" spans="1:22" ht="15">
+    <row r="109" spans="1:22">
       <c r="A109" t="s">
         <v>260</v>
       </c>
@@ -8614,7 +8605,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="110" spans="1:22" ht="15">
+    <row r="110" spans="1:22">
       <c r="A110" t="s">
         <v>260</v>
       </c>
@@ -8661,7 +8652,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="111" spans="1:22" ht="15">
+    <row r="111" spans="1:22">
       <c r="A111" t="s">
         <v>260</v>
       </c>
@@ -8708,7 +8699,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="112" spans="1:22" ht="15">
+    <row r="112" spans="1:22">
       <c r="A112" t="s">
         <v>260</v>
       </c>
@@ -8755,7 +8746,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="113" spans="1:22" ht="15">
+    <row r="113" spans="1:22">
       <c r="A113" t="s">
         <v>260</v>
       </c>
@@ -8802,7 +8793,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="114" spans="1:22" ht="15">
+    <row r="114" spans="1:22">
       <c r="A114" t="s">
         <v>260</v>
       </c>
@@ -8849,7 +8840,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="115" spans="1:22" ht="15">
+    <row r="115" spans="1:22">
       <c r="A115" t="s">
         <v>260</v>
       </c>
@@ -8896,7 +8887,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="116" spans="1:22" ht="15">
+    <row r="116" spans="1:22">
       <c r="A116" t="s">
         <v>260</v>
       </c>
@@ -8943,7 +8934,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="117" spans="1:22" ht="15">
+    <row r="117" spans="1:22">
       <c r="A117" t="s">
         <v>260</v>
       </c>
@@ -8990,7 +8981,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="118" spans="1:22" ht="15">
+    <row r="118" spans="1:22">
       <c r="A118" t="s">
         <v>260</v>
       </c>
@@ -9037,7 +9028,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="119" spans="1:22" ht="15">
+    <row r="119" spans="1:22">
       <c r="A119" t="s">
         <v>260</v>
       </c>
@@ -9084,7 +9075,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="120" spans="1:22" ht="15">
+    <row r="120" spans="1:22">
       <c r="A120" t="s">
         <v>260</v>
       </c>
@@ -9131,7 +9122,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="121" spans="1:22" ht="15">
+    <row r="121" spans="1:22">
       <c r="A121" t="s">
         <v>260</v>
       </c>
@@ -9178,7 +9169,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="122" spans="1:22" ht="15">
+    <row r="122" spans="1:22">
       <c r="A122" t="s">
         <v>260</v>
       </c>
@@ -9225,7 +9216,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="123" spans="1:22" ht="15">
+    <row r="123" spans="1:22">
       <c r="A123" t="s">
         <v>260</v>
       </c>
@@ -9272,7 +9263,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="124" spans="1:22" ht="15">
+    <row r="124" spans="1:22">
       <c r="A124" t="s">
         <v>260</v>
       </c>
@@ -9319,7 +9310,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="125" spans="1:22" ht="15">
+    <row r="125" spans="1:22">
       <c r="A125" t="s">
         <v>260</v>
       </c>
@@ -9366,7 +9357,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="126" spans="1:22" ht="15">
+    <row r="126" spans="1:22">
       <c r="A126" t="s">
         <v>260</v>
       </c>
@@ -9413,7 +9404,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="127" spans="1:22" ht="15">
+    <row r="127" spans="1:22">
       <c r="A127" t="s">
         <v>260</v>
       </c>
@@ -9460,7 +9451,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="128" spans="1:22" ht="15">
+    <row r="128" spans="1:22">
       <c r="A128" t="s">
         <v>260</v>
       </c>
@@ -9507,7 +9498,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="129" spans="1:22" ht="15">
+    <row r="129" spans="1:22">
       <c r="A129" t="s">
         <v>260</v>
       </c>
@@ -9554,7 +9545,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="130" spans="1:22" ht="15">
+    <row r="130" spans="1:22">
       <c r="A130" t="s">
         <v>260</v>
       </c>
@@ -9601,7 +9592,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="131" spans="1:22" ht="15">
+    <row r="131" spans="1:22">
       <c r="A131" t="s">
         <v>260</v>
       </c>
@@ -9648,7 +9639,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="132" spans="1:22" ht="15">
+    <row r="132" spans="1:22">
       <c r="A132" t="s">
         <v>260</v>
       </c>
@@ -9695,7 +9686,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="133" spans="1:22" ht="15">
+    <row r="133" spans="1:22">
       <c r="A133" t="s">
         <v>260</v>
       </c>
@@ -9742,7 +9733,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="134" spans="1:22" ht="15">
+    <row r="134" spans="1:22">
       <c r="A134" t="s">
         <v>260</v>
       </c>
@@ -9789,7 +9780,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="135" spans="1:22" ht="15">
+    <row r="135" spans="1:22">
       <c r="A135" t="s">
         <v>260</v>
       </c>
@@ -9836,7 +9827,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="136" spans="1:22" ht="15">
+    <row r="136" spans="1:22">
       <c r="A136" t="s">
         <v>260</v>
       </c>
@@ -9883,7 +9874,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="137" spans="1:22" ht="15">
+    <row r="137" spans="1:22">
       <c r="A137" t="s">
         <v>260</v>
       </c>
@@ -9930,7 +9921,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="138" spans="1:22" ht="15">
+    <row r="138" spans="1:22">
       <c r="A138" t="s">
         <v>260</v>
       </c>
@@ -9977,7 +9968,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="139" spans="1:22" ht="15">
+    <row r="139" spans="1:22">
       <c r="A139" t="s">
         <v>260</v>
       </c>
@@ -10024,7 +10015,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="140" spans="1:22" ht="15">
+    <row r="140" spans="1:22">
       <c r="A140" t="s">
         <v>260</v>
       </c>
@@ -10071,7 +10062,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="141" spans="1:22" ht="15">
+    <row r="141" spans="1:22">
       <c r="A141" t="s">
         <v>260</v>
       </c>
@@ -10118,7 +10109,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="142" spans="1:22" ht="15">
+    <row r="142" spans="1:22">
       <c r="A142" t="s">
         <v>260</v>
       </c>
@@ -10165,7 +10156,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="143" spans="1:22" ht="15">
+    <row r="143" spans="1:22">
       <c r="A143" t="s">
         <v>260</v>
       </c>
@@ -10212,7 +10203,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="144" spans="1:22" ht="15">
+    <row r="144" spans="1:22">
       <c r="A144" t="s">
         <v>260</v>
       </c>
@@ -10259,7 +10250,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="145" spans="1:22" ht="15">
+    <row r="145" spans="1:22">
       <c r="A145" t="s">
         <v>260</v>
       </c>
@@ -10306,7 +10297,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="146" spans="1:22" ht="15">
+    <row r="146" spans="1:22">
       <c r="A146" t="s">
         <v>260</v>
       </c>
@@ -10353,7 +10344,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="147" spans="1:22" ht="15">
+    <row r="147" spans="1:22">
       <c r="A147" t="s">
         <v>260</v>
       </c>
@@ -10400,7 +10391,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="148" spans="1:22" ht="15">
+    <row r="148" spans="1:22">
       <c r="A148" t="s">
         <v>260</v>
       </c>
@@ -10447,7 +10438,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="149" spans="1:22" ht="15">
+    <row r="149" spans="1:22">
       <c r="A149" t="s">
         <v>260</v>
       </c>
@@ -10494,7 +10485,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="150" spans="1:22" ht="15">
+    <row r="150" spans="1:22">
       <c r="A150" t="s">
         <v>260</v>
       </c>
@@ -10541,7 +10532,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="151" spans="1:22" ht="15">
+    <row r="151" spans="1:22">
       <c r="A151" t="s">
         <v>260</v>
       </c>
@@ -10588,7 +10579,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="152" spans="1:22" ht="15">
+    <row r="152" spans="1:22">
       <c r="A152" t="s">
         <v>260</v>
       </c>
@@ -10635,7 +10626,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="153" spans="1:22" ht="15">
+    <row r="153" spans="1:22">
       <c r="A153" t="s">
         <v>260</v>
       </c>
@@ -10682,7 +10673,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="154" spans="1:22" ht="15">
+    <row r="154" spans="1:22">
       <c r="A154" t="s">
         <v>260</v>
       </c>
@@ -10729,7 +10720,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="155" spans="1:22" ht="15">
+    <row r="155" spans="1:22">
       <c r="A155" t="s">
         <v>260</v>
       </c>
@@ -10776,7 +10767,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="156" spans="1:22" ht="15">
+    <row r="156" spans="1:22">
       <c r="A156" t="s">
         <v>260</v>
       </c>
@@ -10823,7 +10814,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="157" spans="1:22" ht="15">
+    <row r="157" spans="1:22">
       <c r="A157" t="s">
         <v>260</v>
       </c>
@@ -10870,7 +10861,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="158" spans="1:22" ht="15">
+    <row r="158" spans="1:22">
       <c r="A158" t="s">
         <v>260</v>
       </c>
@@ -10917,7 +10908,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="159" spans="1:22" ht="15">
+    <row r="159" spans="1:22">
       <c r="A159" t="s">
         <v>260</v>
       </c>
@@ -10964,7 +10955,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="160" spans="1:22" ht="15">
+    <row r="160" spans="1:22">
       <c r="A160" t="s">
         <v>260</v>
       </c>
@@ -11011,7 +11002,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="161" spans="1:22" ht="15">
+    <row r="161" spans="1:22">
       <c r="A161" t="s">
         <v>260</v>
       </c>
@@ -11058,7 +11049,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="162" spans="1:22" ht="15">
+    <row r="162" spans="1:22">
       <c r="A162" t="s">
         <v>260</v>
       </c>
@@ -11105,7 +11096,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="163" spans="1:22" ht="15">
+    <row r="163" spans="1:22">
       <c r="A163" t="s">
         <v>260</v>
       </c>
@@ -11152,7 +11143,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="164" spans="1:22" ht="15">
+    <row r="164" spans="1:22">
       <c r="A164" t="s">
         <v>260</v>
       </c>
@@ -11199,7 +11190,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="165" spans="1:22" ht="15">
+    <row r="165" spans="1:22">
       <c r="A165" t="s">
         <v>260</v>
       </c>
@@ -11246,7 +11237,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="166" spans="1:22" ht="15">
+    <row r="166" spans="1:22">
       <c r="A166" t="s">
         <v>260</v>
       </c>
@@ -11293,7 +11284,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="167" spans="1:22" ht="15">
+    <row r="167" spans="1:22">
       <c r="A167" t="s">
         <v>260</v>
       </c>
@@ -11340,7 +11331,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="168" spans="1:22" ht="15">
+    <row r="168" spans="1:22">
       <c r="A168" t="s">
         <v>260</v>
       </c>
@@ -11387,7 +11378,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="169" spans="1:22" ht="15">
+    <row r="169" spans="1:22">
       <c r="A169" t="s">
         <v>260</v>
       </c>
@@ -11434,7 +11425,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="170" spans="1:22" ht="15">
+    <row r="170" spans="1:22">
       <c r="A170" t="s">
         <v>260</v>
       </c>
@@ -11481,7 +11472,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="171" spans="1:22" ht="15">
+    <row r="171" spans="1:22">
       <c r="A171" t="s">
         <v>260</v>
       </c>
@@ -11528,7 +11519,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="172" spans="1:22" ht="15">
+    <row r="172" spans="1:22">
       <c r="A172" t="s">
         <v>335</v>
       </c>
@@ -11575,7 +11566,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="173" spans="1:22" ht="15">
+    <row r="173" spans="1:22">
       <c r="A173" t="s">
         <v>335</v>
       </c>
@@ -11622,7 +11613,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="174" spans="1:22" ht="15">
+    <row r="174" spans="1:22">
       <c r="A174" t="s">
         <v>335</v>
       </c>
@@ -11669,7 +11660,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="175" spans="1:22" ht="15">
+    <row r="175" spans="1:22">
       <c r="A175" t="s">
         <v>335</v>
       </c>
@@ -11716,7 +11707,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="176" spans="1:22" ht="15">
+    <row r="176" spans="1:22">
       <c r="A176" t="s">
         <v>335</v>
       </c>
@@ -11763,7 +11754,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="177" spans="1:22" ht="15">
+    <row r="177" spans="1:22">
       <c r="A177" t="s">
         <v>335</v>
       </c>
@@ -11810,7 +11801,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="178" spans="1:22" ht="15">
+    <row r="178" spans="1:22">
       <c r="A178" t="s">
         <v>335</v>
       </c>
@@ -11857,7 +11848,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="179" spans="1:22" ht="15">
+    <row r="179" spans="1:22">
       <c r="A179" t="s">
         <v>335</v>
       </c>
@@ -11904,7 +11895,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="180" spans="1:22" ht="15">
+    <row r="180" spans="1:22">
       <c r="A180" t="s">
         <v>335</v>
       </c>
@@ -11951,7 +11942,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="181" spans="1:22" ht="15">
+    <row r="181" spans="1:22">
       <c r="A181" t="s">
         <v>335</v>
       </c>
@@ -11998,7 +11989,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="182" spans="1:22" ht="15">
+    <row r="182" spans="1:22">
       <c r="A182" t="s">
         <v>335</v>
       </c>
@@ -12045,7 +12036,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="183" spans="1:22" ht="15">
+    <row r="183" spans="1:22">
       <c r="A183" t="s">
         <v>335</v>
       </c>
@@ -12092,7 +12083,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="184" spans="1:22" ht="15">
+    <row r="184" spans="1:22">
       <c r="A184" t="s">
         <v>335</v>
       </c>
@@ -12139,7 +12130,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="185" spans="1:22" ht="15">
+    <row r="185" spans="1:22">
       <c r="A185" t="s">
         <v>335</v>
       </c>
@@ -12186,7 +12177,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="186" spans="1:22" ht="15">
+    <row r="186" spans="1:22">
       <c r="A186" t="s">
         <v>335</v>
       </c>
@@ -12233,7 +12224,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="187" spans="1:22" ht="15">
+    <row r="187" spans="1:22">
       <c r="A187" t="s">
         <v>335</v>
       </c>
@@ -12280,7 +12271,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="188" spans="1:22" ht="15">
+    <row r="188" spans="1:22">
       <c r="A188" t="s">
         <v>335</v>
       </c>
@@ -12327,7 +12318,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="189" spans="1:22" ht="15">
+    <row r="189" spans="1:22">
       <c r="A189" t="s">
         <v>335</v>
       </c>
@@ -12374,7 +12365,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="190" spans="1:22" ht="15">
+    <row r="190" spans="1:22">
       <c r="A190" t="s">
         <v>335</v>
       </c>
@@ -12421,7 +12412,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="191" spans="1:22" ht="15">
+    <row r="191" spans="1:22">
       <c r="A191" t="s">
         <v>335</v>
       </c>
@@ -12468,7 +12459,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="192" spans="1:22" ht="15">
+    <row r="192" spans="1:22">
       <c r="A192" t="s">
         <v>335</v>
       </c>
@@ -12515,7 +12506,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="193" spans="1:25" ht="15">
+    <row r="193" spans="1:25">
       <c r="A193" t="s">
         <v>335</v>
       </c>
@@ -12562,7 +12553,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="194" spans="1:25" ht="15">
+    <row r="194" spans="1:25">
       <c r="A194" t="s">
         <v>358</v>
       </c>
@@ -12618,7 +12609,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="195" spans="1:25" ht="15">
+    <row r="195" spans="1:25">
       <c r="A195" t="s">
         <v>358</v>
       </c>
@@ -12674,7 +12665,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="196" spans="1:25" ht="15">
+    <row r="196" spans="1:25">
       <c r="A196" t="s">
         <v>366</v>
       </c>
@@ -12721,7 +12712,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="197" spans="1:25" ht="15">
+    <row r="197" spans="1:25">
       <c r="A197" t="s">
         <v>370</v>
       </c>
@@ -12768,7 +12759,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="198" spans="1:25" ht="15">
+    <row r="198" spans="1:25">
       <c r="A198" t="s">
         <v>370</v>
       </c>
@@ -12815,7 +12806,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="199" spans="1:25" ht="15">
+    <row r="199" spans="1:25">
       <c r="A199" t="s">
         <v>377</v>
       </c>
@@ -12862,7 +12853,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="200" spans="1:25" ht="15">
+    <row r="200" spans="1:25">
       <c r="A200" t="s">
         <v>377</v>
       </c>
@@ -12909,7 +12900,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="201" spans="1:25" ht="15">
+    <row r="201" spans="1:25">
       <c r="A201" t="s">
         <v>377</v>
       </c>
@@ -12956,7 +12947,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="202" spans="1:25" ht="15">
+    <row r="202" spans="1:25">
       <c r="A202" t="s">
         <v>385</v>
       </c>
@@ -13003,7 +12994,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="203" spans="1:25" ht="15">
+    <row r="203" spans="1:25">
       <c r="A203" t="s">
         <v>385</v>
       </c>
@@ -13047,7 +13038,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="204" spans="1:25" ht="15">
+    <row r="204" spans="1:25">
       <c r="A204" t="s">
         <v>391</v>
       </c>
@@ -13094,7 +13085,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="205" spans="1:25" ht="15">
+    <row r="205" spans="1:25">
       <c r="A205" t="s">
         <v>391</v>
       </c>
@@ -13141,7 +13132,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="206" spans="1:25" ht="15">
+    <row r="206" spans="1:25">
       <c r="A206" t="s">
         <v>391</v>
       </c>
@@ -13188,7 +13179,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="207" spans="1:25" ht="15">
+    <row r="207" spans="1:25">
       <c r="A207" t="s">
         <v>391</v>
       </c>
@@ -13235,7 +13226,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="208" spans="1:25" ht="15">
+    <row r="208" spans="1:25">
       <c r="A208" t="s">
         <v>400</v>
       </c>
@@ -13282,7 +13273,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="209" spans="1:25" ht="15">
+    <row r="209" spans="1:25">
       <c r="A209" t="s">
         <v>404</v>
       </c>
@@ -13335,7 +13326,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="210" spans="1:25" ht="15">
+    <row r="210" spans="1:25">
       <c r="A210" t="s">
         <v>404</v>
       </c>
@@ -13388,7 +13379,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="211" spans="1:25" ht="15">
+    <row r="211" spans="1:25">
       <c r="A211" t="s">
         <v>413</v>
       </c>
@@ -13447,7 +13438,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="212" spans="1:25" ht="15">
+    <row r="212" spans="1:25">
       <c r="A212" t="s">
         <v>413</v>
       </c>
@@ -13506,7 +13497,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="213" spans="1:25" ht="15">
+    <row r="213" spans="1:25">
       <c r="A213" t="s">
         <v>422</v>
       </c>
@@ -13553,7 +13544,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="214" spans="1:25" ht="15">
+    <row r="214" spans="1:25">
       <c r="A214" t="s">
         <v>426</v>
       </c>
@@ -13606,7 +13597,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="215" spans="1:25" ht="15">
+    <row r="215" spans="1:25">
       <c r="A215" t="s">
         <v>426</v>
       </c>
@@ -13659,7 +13650,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="216" spans="1:25" ht="15">
+    <row r="216" spans="1:25">
       <c r="A216" t="s">
         <v>435</v>
       </c>
@@ -13706,7 +13697,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="217" spans="1:25" ht="15">
+    <row r="217" spans="1:25">
       <c r="A217" t="s">
         <v>435</v>
       </c>
@@ -13753,7 +13744,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="218" spans="1:25" ht="15">
+    <row r="218" spans="1:25">
       <c r="A218" t="s">
         <v>440</v>
       </c>
@@ -13800,7 +13791,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="219" spans="1:25" ht="15">
+    <row r="219" spans="1:25">
       <c r="A219" t="s">
         <v>440</v>
       </c>
@@ -13847,7 +13838,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="220" spans="1:25" ht="15">
+    <row r="220" spans="1:25">
       <c r="A220" t="s">
         <v>440</v>
       </c>
@@ -13894,7 +13885,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="221" spans="1:25" ht="15">
+    <row r="221" spans="1:25">
       <c r="A221" t="s">
         <v>440</v>
       </c>
@@ -13941,7 +13932,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="222" spans="1:25" ht="15">
+    <row r="222" spans="1:25">
       <c r="A222" t="s">
         <v>447</v>
       </c>
@@ -13988,7 +13979,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="223" spans="1:25" ht="15">
+    <row r="223" spans="1:25">
       <c r="A223" t="s">
         <v>451</v>
       </c>
@@ -14035,7 +14026,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="224" spans="1:25" ht="15">
+    <row r="224" spans="1:25">
       <c r="A224" t="s">
         <v>451</v>
       </c>
@@ -14082,7 +14073,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="225" spans="1:25" ht="15">
+    <row r="225" spans="1:25">
       <c r="A225" t="s">
         <v>456</v>
       </c>
@@ -14135,7 +14126,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="226" spans="1:25" ht="15">
+    <row r="226" spans="1:25">
       <c r="A226" t="s">
         <v>456</v>
       </c>
@@ -14188,7 +14179,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="227" spans="1:25" ht="15">
+    <row r="227" spans="1:25">
       <c r="A227" t="s">
         <v>465</v>
       </c>
@@ -14244,7 +14235,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="228" spans="1:25" ht="15">
+    <row r="228" spans="1:25">
       <c r="A228" t="s">
         <v>467</v>
       </c>
@@ -14300,7 +14291,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="229" spans="1:25" ht="15">
+    <row r="229" spans="1:25">
       <c r="A229" t="s">
         <v>467</v>
       </c>
@@ -14356,7 +14347,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="230" spans="1:25" ht="15">
+    <row r="230" spans="1:25">
       <c r="A230" t="s">
         <v>467</v>
       </c>
@@ -14412,7 +14403,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="231" spans="1:25" ht="15">
+    <row r="231" spans="1:25">
       <c r="A231" t="s">
         <v>467</v>
       </c>
@@ -14468,7 +14459,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="232" spans="1:25" ht="15">
+    <row r="232" spans="1:25">
       <c r="A232" t="s">
         <v>467</v>
       </c>
@@ -14524,7 +14515,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="233" spans="1:25" ht="15">
+    <row r="233" spans="1:25">
       <c r="A233" t="s">
         <v>467</v>
       </c>
@@ -14580,7 +14571,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="234" spans="1:25" ht="15">
+    <row r="234" spans="1:25">
       <c r="A234" t="s">
         <v>474</v>
       </c>
@@ -14639,7 +14630,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="235" spans="1:25" ht="15">
+    <row r="235" spans="1:25">
       <c r="A235" t="s">
         <v>484</v>
       </c>
@@ -14686,7 +14677,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="236" spans="1:25" ht="15">
+    <row r="236" spans="1:25">
       <c r="A236" t="s">
         <v>487</v>
       </c>
@@ -14733,7 +14724,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="237" spans="1:25" ht="15">
+    <row r="237" spans="1:25">
       <c r="A237" t="s">
         <v>491</v>
       </c>
@@ -14780,7 +14771,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="238" spans="1:25" ht="15">
+    <row r="238" spans="1:25">
       <c r="A238" t="s">
         <v>495</v>
       </c>
@@ -14827,7 +14818,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="239" spans="1:25" ht="15">
+    <row r="239" spans="1:25">
       <c r="A239" t="s">
         <v>495</v>
       </c>
@@ -14874,7 +14865,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="240" spans="1:25" ht="15">
+    <row r="240" spans="1:25">
       <c r="A240" t="s">
         <v>500</v>
       </c>
@@ -14918,7 +14909,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="241" spans="1:25" ht="15">
+    <row r="241" spans="1:25">
       <c r="A241" t="s">
         <v>500</v>
       </c>
@@ -14962,7 +14953,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="242" spans="1:25" ht="15">
+    <row r="242" spans="1:25">
       <c r="A242" t="s">
         <v>500</v>
       </c>
@@ -15009,7 +15000,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="243" spans="1:25" ht="15">
+    <row r="243" spans="1:25">
       <c r="A243" t="s">
         <v>500</v>
       </c>
@@ -15056,7 +15047,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="244" spans="1:25" ht="15">
+    <row r="244" spans="1:25">
       <c r="A244" t="s">
         <v>508</v>
       </c>
@@ -15100,7 +15091,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="245" spans="1:25" ht="15">
+    <row r="245" spans="1:25">
       <c r="A245" t="s">
         <v>508</v>
       </c>
@@ -15144,7 +15135,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="246" spans="1:25" ht="15">
+    <row r="246" spans="1:25">
       <c r="A246" t="s">
         <v>512</v>
       </c>
@@ -15191,7 +15182,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="247" spans="1:25" ht="15">
+    <row r="247" spans="1:25">
       <c r="A247" t="s">
         <v>512</v>
       </c>
@@ -15238,7 +15229,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="248" spans="1:25" ht="15">
+    <row r="248" spans="1:25">
       <c r="A248" t="s">
         <v>512</v>
       </c>
@@ -15285,7 +15276,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="249" spans="1:25" ht="15">
+    <row r="249" spans="1:25">
       <c r="A249" t="s">
         <v>512</v>
       </c>
@@ -15332,7 +15323,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="250" spans="1:25" ht="15">
+    <row r="250" spans="1:25">
       <c r="A250" t="s">
         <v>519</v>
       </c>
@@ -15379,7 +15370,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="251" spans="1:25" ht="15">
+    <row r="251" spans="1:25">
       <c r="A251" t="s">
         <v>519</v>
       </c>
@@ -15426,7 +15417,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="252" spans="1:25" ht="15">
+    <row r="252" spans="1:25">
       <c r="A252" t="s">
         <v>519</v>
       </c>
@@ -15473,7 +15464,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="253" spans="1:25" ht="15">
+    <row r="253" spans="1:25">
       <c r="A253" t="s">
         <v>519</v>
       </c>
@@ -15520,7 +15511,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="254" spans="1:25" ht="15">
+    <row r="254" spans="1:25">
       <c r="A254" t="s">
         <v>526</v>
       </c>
@@ -15567,7 +15558,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="255" spans="1:25" ht="15">
+    <row r="255" spans="1:25">
       <c r="A255" t="s">
         <v>529</v>
       </c>
@@ -15620,7 +15611,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="256" spans="1:25" ht="15">
+    <row r="256" spans="1:25">
       <c r="A256" t="s">
         <v>529</v>
       </c>
@@ -15673,7 +15664,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="257" spans="1:25" ht="15">
+    <row r="257" spans="1:25">
       <c r="A257" t="s">
         <v>536</v>
       </c>
@@ -15732,7 +15723,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="258" spans="1:25" ht="15">
+    <row r="258" spans="1:25">
       <c r="A258" t="s">
         <v>544</v>
       </c>
@@ -15788,7 +15779,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="259" spans="1:25" ht="15">
+    <row r="259" spans="1:25">
       <c r="A259" t="s">
         <v>544</v>
       </c>
@@ -15844,7 +15835,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="260" spans="1:25" ht="15">
+    <row r="260" spans="1:25">
       <c r="A260" t="s">
         <v>544</v>
       </c>
@@ -15900,7 +15891,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="261" spans="1:25" ht="15">
+    <row r="261" spans="1:25">
       <c r="A261" t="s">
         <v>544</v>
       </c>
@@ -15956,7 +15947,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="262" spans="1:25" ht="15">
+    <row r="262" spans="1:25">
       <c r="A262" t="s">
         <v>544</v>
       </c>
@@ -16012,7 +16003,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="263" spans="1:25" ht="15">
+    <row r="263" spans="1:25">
       <c r="A263" t="s">
         <v>544</v>
       </c>
@@ -16068,7 +16059,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="264" spans="1:25" ht="15">
+    <row r="264" spans="1:25">
       <c r="A264" t="s">
         <v>544</v>
       </c>
@@ -16124,7 +16115,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="265" spans="1:25" ht="15">
+    <row r="265" spans="1:25">
       <c r="A265" t="s">
         <v>557</v>
       </c>
@@ -16183,7 +16174,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="266" spans="1:25" ht="15">
+    <row r="266" spans="1:25">
       <c r="A266" t="s">
         <v>567</v>
       </c>
@@ -16236,7 +16227,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="267" spans="1:25" ht="15">
+    <row r="267" spans="1:25">
       <c r="A267" t="s">
         <v>574</v>
       </c>
@@ -16283,7 +16274,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="268" spans="1:25" ht="15">
+    <row r="268" spans="1:25">
       <c r="A268" t="s">
         <v>574</v>
       </c>
@@ -16330,7 +16321,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="269" spans="1:25" ht="15">
+    <row r="269" spans="1:25">
       <c r="A269" t="s">
         <v>574</v>
       </c>
@@ -16377,7 +16368,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="270" spans="1:25" ht="15">
+    <row r="270" spans="1:25">
       <c r="A270" t="s">
         <v>574</v>
       </c>
@@ -16424,7 +16415,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="271" spans="1:25" ht="15">
+    <row r="271" spans="1:25">
       <c r="A271" t="s">
         <v>579</v>
       </c>
@@ -16474,7 +16465,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="272" spans="1:25" ht="15">
+    <row r="272" spans="1:25">
       <c r="A272" t="s">
         <v>579</v>
       </c>
@@ -16524,7 +16515,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="273" spans="1:25" ht="15">
+    <row r="273" spans="1:25">
       <c r="A273" t="s">
         <v>584</v>
       </c>
@@ -16568,7 +16559,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="274" spans="1:25" ht="15">
+    <row r="274" spans="1:25">
       <c r="A274" t="s">
         <v>587</v>
       </c>
@@ -16627,7 +16618,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="275" spans="1:25" ht="15">
+    <row r="275" spans="1:25">
       <c r="A275" t="s">
         <v>587</v>
       </c>
@@ -16686,7 +16677,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="276" spans="1:25" ht="15">
+    <row r="276" spans="1:25">
       <c r="A276" t="s">
         <v>597</v>
       </c>
@@ -16745,7 +16736,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="277" spans="1:25" ht="15">
+    <row r="277" spans="1:25">
       <c r="A277" t="s">
         <v>597</v>
       </c>
@@ -16798,7 +16789,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="278" spans="1:25" ht="15">
+    <row r="278" spans="1:25">
       <c r="A278" t="s">
         <v>606</v>
       </c>
@@ -16854,7 +16845,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="279" spans="1:25" ht="15">
+    <row r="279" spans="1:25">
       <c r="A279" t="s">
         <v>606</v>
       </c>
@@ -16910,7 +16901,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="280" spans="1:25" ht="15">
+    <row r="280" spans="1:25">
       <c r="A280" t="s">
         <v>606</v>
       </c>
@@ -16966,7 +16957,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="281" spans="1:25" ht="15">
+    <row r="281" spans="1:25">
       <c r="A281" t="s">
         <v>615</v>
       </c>
@@ -17016,7 +17007,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="282" spans="1:25" ht="15">
+    <row r="282" spans="1:25">
       <c r="A282" t="s">
         <v>615</v>
       </c>
@@ -17066,7 +17057,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="283" spans="1:25" ht="15">
+    <row r="283" spans="1:25">
       <c r="A283" t="s">
         <v>620</v>
       </c>
@@ -17116,7 +17107,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="284" spans="1:25" ht="15">
+    <row r="284" spans="1:25">
       <c r="A284" t="s">
         <v>620</v>
       </c>
@@ -17166,7 +17157,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="285" spans="1:25" ht="15">
+    <row r="285" spans="1:25">
       <c r="A285" t="s">
         <v>620</v>
       </c>
@@ -17216,7 +17207,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="286" spans="1:25" ht="15">
+    <row r="286" spans="1:25">
       <c r="A286" t="s">
         <v>620</v>
       </c>
@@ -17266,7 +17257,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="287" spans="1:25" ht="15">
+    <row r="287" spans="1:25">
       <c r="A287" t="s">
         <v>627</v>
       </c>
@@ -17316,7 +17307,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="288" spans="1:25" ht="15">
+    <row r="288" spans="1:25">
       <c r="A288" t="s">
         <v>627</v>
       </c>
@@ -17366,7 +17357,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="289" spans="1:22" ht="15">
+    <row r="289" spans="1:22">
       <c r="A289" t="s">
         <v>627</v>
       </c>
@@ -17416,7 +17407,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="290" spans="1:22" ht="15">
+    <row r="290" spans="1:22">
       <c r="A290" t="s">
         <v>627</v>
       </c>
@@ -17466,7 +17457,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="291" spans="1:22" ht="15">
+    <row r="291" spans="1:22">
       <c r="A291" t="s">
         <v>627</v>
       </c>
@@ -17516,7 +17507,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="292" spans="1:22" ht="15">
+    <row r="292" spans="1:22">
       <c r="A292" t="s">
         <v>627</v>
       </c>
@@ -17566,7 +17557,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="293" spans="1:22" ht="15">
+    <row r="293" spans="1:22">
       <c r="A293" t="s">
         <v>636</v>
       </c>
@@ -17613,7 +17604,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="294" spans="1:22" ht="15">
+    <row r="294" spans="1:22">
       <c r="A294" t="s">
         <v>636</v>
       </c>
@@ -17660,7 +17651,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="295" spans="1:22" ht="15">
+    <row r="295" spans="1:22">
       <c r="A295" t="s">
         <v>636</v>
       </c>
@@ -17707,7 +17698,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="296" spans="1:22" ht="15">
+    <row r="296" spans="1:22">
       <c r="A296" t="s">
         <v>636</v>
       </c>
@@ -17754,7 +17745,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="297" spans="1:22" ht="15">
+    <row r="297" spans="1:22">
       <c r="A297" t="s">
         <v>642</v>
       </c>
@@ -17798,7 +17789,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="298" spans="1:22" ht="15">
+    <row r="298" spans="1:22">
       <c r="A298" t="s">
         <v>642</v>
       </c>
@@ -17842,7 +17833,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="299" spans="1:22" ht="15">
+    <row r="299" spans="1:22">
       <c r="A299" t="s">
         <v>646</v>
       </c>
@@ -17889,7 +17880,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="300" spans="1:22" ht="15">
+    <row r="300" spans="1:22">
       <c r="A300" t="s">
         <v>646</v>
       </c>
@@ -17936,7 +17927,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="301" spans="1:22" ht="15">
+    <row r="301" spans="1:22">
       <c r="A301" t="s">
         <v>651</v>
       </c>
@@ -17983,7 +17974,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="302" spans="1:22" ht="15">
+    <row r="302" spans="1:22">
       <c r="A302" t="s">
         <v>651</v>
       </c>
@@ -18030,7 +18021,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="303" spans="1:22" ht="15">
+    <row r="303" spans="1:22">
       <c r="A303" t="s">
         <v>654</v>
       </c>
@@ -18077,7 +18068,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="304" spans="1:22" ht="15">
+    <row r="304" spans="1:22">
       <c r="A304" t="s">
         <v>654</v>
       </c>
@@ -18124,7 +18115,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="305" spans="1:25" ht="15">
+    <row r="305" spans="1:25">
       <c r="A305" t="s">
         <v>659</v>
       </c>
@@ -18171,7 +18162,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="306" spans="1:25" ht="15">
+    <row r="306" spans="1:25">
       <c r="A306" t="s">
         <v>659</v>
       </c>
@@ -18218,7 +18209,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="307" spans="1:25" ht="15">
+    <row r="307" spans="1:25">
       <c r="A307" t="s">
         <v>659</v>
       </c>
@@ -18265,7 +18256,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="308" spans="1:25" ht="15">
+    <row r="308" spans="1:25">
       <c r="A308" t="s">
         <v>659</v>
       </c>
@@ -18312,7 +18303,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="309" spans="1:25" ht="15">
+    <row r="309" spans="1:25">
       <c r="A309" t="s">
         <v>659</v>
       </c>
@@ -18359,7 +18350,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="310" spans="1:25" ht="15">
+    <row r="310" spans="1:25">
       <c r="A310" t="s">
         <v>659</v>
       </c>
@@ -18406,7 +18397,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="311" spans="1:25" ht="15">
+    <row r="311" spans="1:25">
       <c r="A311" t="s">
         <v>659</v>
       </c>
@@ -18453,7 +18444,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="312" spans="1:25" ht="15">
+    <row r="312" spans="1:25">
       <c r="A312" t="s">
         <v>659</v>
       </c>
@@ -18500,7 +18491,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="313" spans="1:25" ht="15">
+    <row r="313" spans="1:25">
       <c r="A313" t="s">
         <v>659</v>
       </c>
@@ -18547,7 +18538,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="314" spans="1:25" ht="15">
+    <row r="314" spans="1:25">
       <c r="A314" t="s">
         <v>659</v>
       </c>
@@ -18594,7 +18585,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="315" spans="1:25" ht="15">
+    <row r="315" spans="1:25">
       <c r="A315" t="s">
         <v>671</v>
       </c>
@@ -18644,7 +18635,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="316" spans="1:25" ht="15">
+    <row r="316" spans="1:25">
       <c r="A316" t="s">
         <v>671</v>
       </c>
@@ -18694,7 +18685,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="317" spans="1:25" ht="15">
+    <row r="317" spans="1:25">
       <c r="A317" t="s">
         <v>671</v>
       </c>
@@ -18744,7 +18735,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="318" spans="1:25" ht="15">
+    <row r="318" spans="1:25">
       <c r="A318" t="s">
         <v>671</v>
       </c>
@@ -18794,7 +18785,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="319" spans="1:25" ht="15">
+    <row r="319" spans="1:25">
       <c r="A319" t="s">
         <v>671</v>
       </c>
@@ -18844,7 +18835,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="320" spans="1:25" ht="15">
+    <row r="320" spans="1:25">
       <c r="A320" t="s">
         <v>671</v>
       </c>
@@ -18894,7 +18885,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="321" spans="1:25" ht="15">
+    <row r="321" spans="1:25">
       <c r="A321" t="s">
         <v>682</v>
       </c>
@@ -18947,7 +18938,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="322" spans="1:25" ht="15">
+    <row r="322" spans="1:25">
       <c r="A322" t="s">
         <v>689</v>
       </c>
@@ -18994,7 +18985,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="323" spans="1:25" ht="15">
+    <row r="323" spans="1:25">
       <c r="A323" t="s">
         <v>689</v>
       </c>
@@ -19041,7 +19032,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="324" spans="1:25" ht="15">
+    <row r="324" spans="1:25">
       <c r="A324" t="s">
         <v>694</v>
       </c>
@@ -19100,7 +19091,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="325" spans="1:25" ht="15">
+    <row r="325" spans="1:25">
       <c r="A325" t="s">
         <v>694</v>
       </c>
@@ -19159,7 +19150,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="326" spans="1:25" ht="15">
+    <row r="326" spans="1:25">
       <c r="A326" t="s">
         <v>702</v>
       </c>
@@ -19212,7 +19203,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="327" spans="1:25" ht="15">
+    <row r="327" spans="1:25">
       <c r="A327" t="s">
         <v>702</v>
       </c>
@@ -19265,7 +19256,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="328" spans="1:25" ht="15">
+    <row r="328" spans="1:25">
       <c r="A328" t="s">
         <v>709</v>
       </c>
@@ -19321,7 +19312,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="329" spans="1:25" ht="15">
+    <row r="329" spans="1:25">
       <c r="A329" t="s">
         <v>716</v>
       </c>
@@ -19374,7 +19365,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="330" spans="1:25" ht="15">
+    <row r="330" spans="1:25">
       <c r="A330" t="s">
         <v>723</v>
       </c>
@@ -19427,7 +19418,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="331" spans="1:25" ht="15">
+    <row r="331" spans="1:25">
       <c r="A331" t="s">
         <v>730</v>
       </c>
@@ -19474,7 +19465,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="332" spans="1:25" ht="15">
+    <row r="332" spans="1:25">
       <c r="A332" t="s">
         <v>730</v>
       </c>
@@ -19521,7 +19512,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="333" spans="1:25" ht="15">
+    <row r="333" spans="1:25">
       <c r="A333" t="s">
         <v>730</v>
       </c>
@@ -19568,7 +19559,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="334" spans="1:25" ht="15">
+    <row r="334" spans="1:25">
       <c r="A334" t="s">
         <v>730</v>
       </c>
@@ -19615,7 +19606,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="335" spans="1:25" ht="15">
+    <row r="335" spans="1:25">
       <c r="A335" t="s">
         <v>730</v>
       </c>
@@ -19662,7 +19653,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="336" spans="1:25" ht="15">
+    <row r="336" spans="1:25">
       <c r="A336" t="s">
         <v>730</v>
       </c>
@@ -19709,7 +19700,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="337" spans="1:25" ht="15">
+    <row r="337" spans="1:25">
       <c r="A337" t="s">
         <v>730</v>
       </c>
@@ -19756,7 +19747,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="338" spans="1:25" ht="15">
+    <row r="338" spans="1:25">
       <c r="A338" t="s">
         <v>730</v>
       </c>
@@ -19803,7 +19794,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="339" spans="1:25" ht="15">
+    <row r="339" spans="1:25">
       <c r="A339" t="s">
         <v>739</v>
       </c>
@@ -19847,7 +19838,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="340" spans="1:25" ht="15">
+    <row r="340" spans="1:25">
       <c r="A340" t="s">
         <v>739</v>
       </c>
@@ -19891,7 +19882,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="341" spans="1:25" ht="15">
+    <row r="341" spans="1:25">
       <c r="A341" t="s">
         <v>744</v>
       </c>
@@ -19938,7 +19929,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="342" spans="1:25" ht="15">
+    <row r="342" spans="1:25">
       <c r="A342" t="s">
         <v>744</v>
       </c>
@@ -19985,7 +19976,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="343" spans="1:25" ht="15">
+    <row r="343" spans="1:25">
       <c r="A343" t="s">
         <v>749</v>
       </c>
@@ -20035,7 +20026,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="344" spans="1:25" ht="15">
+    <row r="344" spans="1:25">
       <c r="A344" t="s">
         <v>749</v>
       </c>
@@ -20085,7 +20076,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="345" spans="1:25" ht="15">
+    <row r="345" spans="1:25">
       <c r="A345" t="s">
         <v>752</v>
       </c>
@@ -20144,7 +20135,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="346" spans="1:25" ht="15">
+    <row r="346" spans="1:25">
       <c r="A346" t="s">
         <v>752</v>
       </c>
@@ -20203,7 +20194,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="347" spans="1:25" ht="15">
+    <row r="347" spans="1:25">
       <c r="A347" t="s">
         <v>752</v>
       </c>
@@ -20256,7 +20247,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="348" spans="1:25" ht="15">
+    <row r="348" spans="1:25">
       <c r="A348" t="s">
         <v>752</v>
       </c>
@@ -20309,7 +20300,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="349" spans="1:25" ht="15">
+    <row r="349" spans="1:25">
       <c r="A349" t="s">
         <v>763</v>
       </c>
@@ -20359,7 +20350,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="350" spans="1:25" ht="15">
+    <row r="350" spans="1:25">
       <c r="A350" t="s">
         <v>763</v>
       </c>
@@ -20409,7 +20400,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="351" spans="1:25" ht="15">
+    <row r="351" spans="1:25">
       <c r="A351" t="s">
         <v>770</v>
       </c>
@@ -20468,7 +20459,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="352" spans="1:25" ht="15">
+    <row r="352" spans="1:25">
       <c r="A352" t="s">
         <v>770</v>
       </c>
@@ -20527,7 +20518,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="353" spans="1:25" ht="15">
+    <row r="353" spans="1:25">
       <c r="A353" t="s">
         <v>778</v>
       </c>
@@ -20577,7 +20568,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="354" spans="1:25" ht="15">
+    <row r="354" spans="1:25">
       <c r="A354" t="s">
         <v>778</v>
       </c>
@@ -20627,7 +20618,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="355" spans="1:25" ht="15">
+    <row r="355" spans="1:25">
       <c r="A355" t="s">
         <v>783</v>
       </c>
@@ -20674,7 +20665,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="356" spans="1:25" ht="15">
+    <row r="356" spans="1:25">
       <c r="A356" t="s">
         <v>783</v>
       </c>
@@ -20721,7 +20712,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="357" spans="1:25" ht="15">
+    <row r="357" spans="1:25">
       <c r="A357" t="s">
         <v>788</v>
       </c>
@@ -20777,7 +20768,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="358" spans="1:25" ht="15">
+    <row r="358" spans="1:25">
       <c r="A358" t="s">
         <v>796</v>
       </c>
@@ -20824,7 +20815,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="359" spans="1:25" ht="15">
+    <row r="359" spans="1:25">
       <c r="A359" t="s">
         <v>796</v>
       </c>
@@ -20871,7 +20862,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="360" spans="1:25" ht="15">
+    <row r="360" spans="1:25">
       <c r="A360" t="s">
         <v>796</v>
       </c>
@@ -20918,7 +20909,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="361" spans="1:25" ht="15">
+    <row r="361" spans="1:25">
       <c r="A361" t="s">
         <v>796</v>
       </c>
@@ -20965,7 +20956,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="362" spans="1:25" ht="15">
+    <row r="362" spans="1:25">
       <c r="A362" t="s">
         <v>796</v>
       </c>
@@ -21012,7 +21003,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="363" spans="1:25" ht="15">
+    <row r="363" spans="1:25">
       <c r="A363" t="s">
         <v>796</v>
       </c>
@@ -21059,7 +21050,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="364" spans="1:25" ht="15">
+    <row r="364" spans="1:25">
       <c r="A364" t="s">
         <v>796</v>
       </c>
@@ -21106,7 +21097,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="365" spans="1:25" ht="15">
+    <row r="365" spans="1:25">
       <c r="A365" t="s">
         <v>796</v>
       </c>
@@ -21153,7 +21144,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="366" spans="1:25" ht="15">
+    <row r="366" spans="1:25">
       <c r="A366" t="s">
         <v>796</v>
       </c>
@@ -21200,7 +21191,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="367" spans="1:25" ht="15">
+    <row r="367" spans="1:25">
       <c r="A367" t="s">
         <v>796</v>
       </c>
@@ -21247,7 +21238,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="368" spans="1:25" ht="15">
+    <row r="368" spans="1:25">
       <c r="A368" t="s">
         <v>808</v>
       </c>
@@ -21291,7 +21282,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="369" spans="1:22" ht="15">
+    <row r="369" spans="1:22">
       <c r="A369" t="s">
         <v>808</v>
       </c>
@@ -21335,7 +21326,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="370" spans="1:22" ht="15">
+    <row r="370" spans="1:22">
       <c r="A370" t="s">
         <v>812</v>
       </c>
@@ -21385,7 +21376,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="371" spans="1:22" ht="15">
+    <row r="371" spans="1:22">
       <c r="A371" t="s">
         <v>812</v>
       </c>
@@ -21435,7 +21426,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="372" spans="1:22" ht="15">
+    <row r="372" spans="1:22">
       <c r="A372" t="s">
         <v>812</v>
       </c>
@@ -21485,7 +21476,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="373" spans="1:22" ht="15">
+    <row r="373" spans="1:22">
       <c r="A373" t="s">
         <v>812</v>
       </c>
@@ -21535,7 +21526,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="374" spans="1:22" ht="15">
+    <row r="374" spans="1:22">
       <c r="A374" t="s">
         <v>812</v>
       </c>
@@ -21585,7 +21576,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="375" spans="1:22" ht="15">
+    <row r="375" spans="1:22">
       <c r="A375" t="s">
         <v>812</v>
       </c>
@@ -21635,7 +21626,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="376" spans="1:22" ht="15">
+    <row r="376" spans="1:22">
       <c r="A376" t="s">
         <v>821</v>
       </c>
@@ -21685,7 +21676,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="377" spans="1:22" ht="15">
+    <row r="377" spans="1:22">
       <c r="A377" t="s">
         <v>821</v>
       </c>
@@ -21735,7 +21726,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="378" spans="1:22" ht="15">
+    <row r="378" spans="1:22">
       <c r="A378" t="s">
         <v>821</v>
       </c>
@@ -21785,7 +21776,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="379" spans="1:22" ht="15">
+    <row r="379" spans="1:22">
       <c r="A379" t="s">
         <v>821</v>
       </c>
@@ -21835,7 +21826,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="380" spans="1:22" ht="15">
+    <row r="380" spans="1:22">
       <c r="A380" t="s">
         <v>826</v>
       </c>
@@ -21879,7 +21870,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="381" spans="1:22" ht="15">
+    <row r="381" spans="1:22">
       <c r="A381" t="s">
         <v>826</v>
       </c>
@@ -21923,7 +21914,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="382" spans="1:22" ht="15">
+    <row r="382" spans="1:22">
       <c r="A382" t="s">
         <v>826</v>
       </c>
@@ -21970,7 +21961,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="383" spans="1:22" ht="15">
+    <row r="383" spans="1:22">
       <c r="A383" t="s">
         <v>826</v>
       </c>
@@ -22017,7 +22008,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="384" spans="1:22" ht="15">
+    <row r="384" spans="1:22">
       <c r="A384" t="s">
         <v>834</v>
       </c>
@@ -22064,7 +22055,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="385" spans="1:25" ht="15">
+    <row r="385" spans="1:25">
       <c r="A385" t="s">
         <v>834</v>
       </c>
@@ -22111,7 +22102,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="386" spans="1:25" ht="15">
+    <row r="386" spans="1:25">
       <c r="A386" t="s">
         <v>834</v>
       </c>
@@ -22158,7 +22149,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="387" spans="1:25" ht="15">
+    <row r="387" spans="1:25">
       <c r="A387" t="s">
         <v>834</v>
       </c>
@@ -22205,7 +22196,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="388" spans="1:25" ht="15">
+    <row r="388" spans="1:25">
       <c r="A388" t="s">
         <v>843</v>
       </c>
@@ -22249,7 +22240,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="389" spans="1:25" ht="15">
+    <row r="389" spans="1:25">
       <c r="A389" t="s">
         <v>843</v>
       </c>
@@ -22293,7 +22284,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="390" spans="1:25" ht="15">
+    <row r="390" spans="1:25">
       <c r="A390" t="s">
         <v>847</v>
       </c>
@@ -22340,7 +22331,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="391" spans="1:25" ht="15">
+    <row r="391" spans="1:25">
       <c r="A391" t="s">
         <v>850</v>
       </c>
@@ -22393,7 +22384,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="392" spans="1:25" ht="15">
+    <row r="392" spans="1:25">
       <c r="A392" t="s">
         <v>857</v>
       </c>
@@ -22446,7 +22437,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="393" spans="1:25" ht="15">
+    <row r="393" spans="1:25">
       <c r="A393" t="s">
         <v>857</v>
       </c>
@@ -22499,7 +22490,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="394" spans="1:25" ht="15">
+    <row r="394" spans="1:25">
       <c r="A394" t="s">
         <v>865</v>
       </c>
@@ -22552,7 +22543,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="395" spans="1:25" ht="15">
+    <row r="395" spans="1:25">
       <c r="A395" t="s">
         <v>867</v>
       </c>
@@ -22614,7 +22605,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="396" spans="1:25" ht="15">
+    <row r="396" spans="1:25">
       <c r="A396" t="s">
         <v>867</v>
       </c>
@@ -22670,7 +22661,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="397" spans="1:25" ht="15">
+    <row r="397" spans="1:25">
       <c r="A397" t="s">
         <v>874</v>
       </c>
@@ -22726,7 +22717,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="398" spans="1:25" ht="15">
+    <row r="398" spans="1:25">
       <c r="A398" t="s">
         <v>874</v>
       </c>
@@ -22782,7 +22773,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="399" spans="1:25" ht="15">
+    <row r="399" spans="1:25">
       <c r="A399" t="s">
         <v>874</v>
       </c>
@@ -22841,7 +22832,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="400" spans="1:25" ht="15">
+    <row r="400" spans="1:25">
       <c r="A400" t="s">
         <v>884</v>
       </c>
@@ -22888,7 +22879,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="401" spans="1:25" ht="15">
+    <row r="401" spans="1:25">
       <c r="A401" t="s">
         <v>884</v>
       </c>
@@ -22935,7 +22926,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="402" spans="1:25" ht="15">
+    <row r="402" spans="1:25">
       <c r="A402" t="s">
         <v>884</v>
       </c>
@@ -22982,7 +22973,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="403" spans="1:25" ht="15">
+    <row r="403" spans="1:25">
       <c r="A403" t="s">
         <v>884</v>
       </c>
@@ -23029,7 +23020,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="404" spans="1:25" ht="15">
+    <row r="404" spans="1:25">
       <c r="A404" t="s">
         <v>891</v>
       </c>
@@ -23085,7 +23076,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="405" spans="1:25" ht="15">
+    <row r="405" spans="1:25">
       <c r="A405" t="s">
         <v>891</v>
       </c>
@@ -23141,7 +23132,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="406" spans="1:25" ht="15">
+    <row r="406" spans="1:25">
       <c r="A406" t="s">
         <v>900</v>
       </c>
@@ -23197,7 +23188,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="407" spans="1:25" ht="15">
+    <row r="407" spans="1:25">
       <c r="A407" t="s">
         <v>907</v>
       </c>
@@ -23250,7 +23241,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="408" spans="1:25" ht="15">
+    <row r="408" spans="1:25">
       <c r="A408" t="s">
         <v>907</v>
       </c>
@@ -23303,7 +23294,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="409" spans="1:25" ht="15">
+    <row r="409" spans="1:25">
       <c r="A409" t="s">
         <v>916</v>
       </c>
@@ -23359,7 +23350,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="410" spans="1:25" ht="15">
+    <row r="410" spans="1:25">
       <c r="A410" t="s">
         <v>916</v>
       </c>
@@ -23415,7 +23406,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="411" spans="1:25" ht="15">
+    <row r="411" spans="1:25">
       <c r="A411" t="s">
         <v>924</v>
       </c>
@@ -23471,7 +23462,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="412" spans="1:25" ht="15">
+    <row r="412" spans="1:25">
       <c r="A412" t="s">
         <v>924</v>
       </c>
@@ -23527,7 +23518,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="413" spans="1:25" ht="15">
+    <row r="413" spans="1:25">
       <c r="A413" t="s">
         <v>933</v>
       </c>
@@ -23586,7 +23577,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="414" spans="1:25" ht="15">
+    <row r="414" spans="1:25">
       <c r="A414" t="s">
         <v>933</v>
       </c>
@@ -23645,7 +23636,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="415" spans="1:25" ht="15">
+    <row r="415" spans="1:25">
       <c r="A415" t="s">
         <v>933</v>
       </c>
@@ -23704,7 +23695,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="416" spans="1:25" ht="15">
+    <row r="416" spans="1:25">
       <c r="A416" t="s">
         <v>933</v>
       </c>
@@ -23763,7 +23754,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="417" spans="1:25" ht="15">
+    <row r="417" spans="1:25">
       <c r="A417" t="s">
         <v>933</v>
       </c>
@@ -23822,7 +23813,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="418" spans="1:25" ht="15">
+    <row r="418" spans="1:25">
       <c r="A418" t="s">
         <v>945</v>
       </c>
@@ -23875,7 +23866,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="419" spans="1:25" ht="15">
+    <row r="419" spans="1:25">
       <c r="A419" t="s">
         <v>945</v>
       </c>
@@ -23928,7 +23919,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="420" spans="1:25" ht="15">
+    <row r="420" spans="1:25">
       <c r="A420" t="s">
         <v>945</v>
       </c>
@@ -23981,7 +23972,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="421" spans="1:25" ht="15">
+    <row r="421" spans="1:25">
       <c r="A421" t="s">
         <v>954</v>
       </c>
@@ -24028,7 +24019,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="422" spans="1:25" ht="15">
+    <row r="422" spans="1:25">
       <c r="A422" t="s">
         <v>961</v>
       </c>
@@ -24075,7 +24066,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="423" spans="1:25" ht="15">
+    <row r="423" spans="1:25">
       <c r="A423" t="s">
         <v>965</v>
       </c>
@@ -24125,7 +24116,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="424" spans="1:25" ht="15">
+    <row r="424" spans="1:25">
       <c r="A424" t="s">
         <v>969</v>
       </c>
@@ -24175,7 +24166,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="425" spans="1:25" ht="15">
+    <row r="425" spans="1:25">
       <c r="A425" t="s">
         <v>969</v>
       </c>
@@ -24225,7 +24216,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="426" spans="1:25" ht="15">
+    <row r="426" spans="1:25">
       <c r="A426" t="s">
         <v>969</v>
       </c>
@@ -24275,7 +24266,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="427" spans="1:25" ht="15">
+    <row r="427" spans="1:25">
       <c r="A427" t="s">
         <v>969</v>
       </c>
@@ -24325,7 +24316,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="428" spans="1:25" ht="15">
+    <row r="428" spans="1:25">
       <c r="A428" t="s">
         <v>969</v>
       </c>
@@ -24375,7 +24366,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="429" spans="1:25" ht="15">
+    <row r="429" spans="1:25">
       <c r="A429" t="s">
         <v>969</v>
       </c>
@@ -24425,7 +24416,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="430" spans="1:25" ht="15">
+    <row r="430" spans="1:25">
       <c r="A430" t="s">
         <v>969</v>
       </c>
@@ -24475,7 +24466,7 @@
         <v>97223</v>
       </c>
     </row>
-    <row r="431" spans="1:25" ht="15">
+    <row r="431" spans="1:25">
       <c r="A431" t="s">
         <v>979</v>
       </c>
@@ -24528,7 +24519,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="432" spans="1:25" ht="15">
+    <row r="432" spans="1:25">
       <c r="A432" t="s">
         <v>979</v>
       </c>
@@ -24582,10 +24573,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:Y1"/>
-  </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>